<commit_message>
Add extra point for use of semantic elements in 'index.html'
</commit_message>
<xml_diff>
--- a/GradedExercise.xlsx
+++ b/GradedExercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianr/Temp/fs19-de-graded-exercise-05-28-2019-02-13-11/mzhKU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1151B3-BB39-8744-A036-284F2C9E70F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61105A25-C46B-DC4E-B186-F5AAE025DAEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3160" yWindow="460" windowWidth="30440" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>It works</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>Module name can be empty, NOT complete</t>
+  </si>
+  <si>
+    <t>Use of semantic elements in index.html</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
   <dimension ref="B1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1022,10 @@
         <v>20</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
@@ -1031,11 +1037,11 @@
       </c>
       <c r="G30" s="3">
         <f>SUM(G25:G29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="3">
         <f>MIN(C30,G30)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
@@ -1051,7 +1057,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="10">
         <f>SUM(H4:H30)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
@@ -1113,7 +1119,7 @@
       <c r="H40" s="9"/>
       <c r="I40" s="9">
         <f>Bonus-Malus</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
@@ -1128,7 +1134,7 @@
       <c r="H42" s="4"/>
       <c r="I42" s="5">
         <f>1 + TOTAL/10</f>
-        <v>5.4</v>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>